<commit_message>
complete excel data class add simple code for business and presentation tiers
</commit_message>
<xml_diff>
--- a/Draft/Presentation/Run_TestCase/TestCases.xlsx
+++ b/Draft/Presentation/Run_TestCase/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -85,15 +85,6 @@
     <t>btn</t>
   </si>
   <si>
-    <t>navigate</t>
-  </si>
-  <si>
-    <t>input</t>
-  </si>
-  <si>
-    <t>click</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -113,6 +104,12 @@
   </si>
   <si>
     <t>XPath</t>
+  </si>
+  <si>
+    <t>Navigate</t>
+  </si>
+  <si>
+    <t>Click</t>
   </si>
 </sst>
 </file>
@@ -478,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +518,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -552,7 +549,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -570,7 +567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -586,7 +583,7 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -595,10 +592,10 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s">
         <v>9</v>
@@ -612,7 +609,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -629,7 +626,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -643,16 +640,16 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
         <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
       </c>
       <c r="G4" t="s">
         <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add selenium web driver
</commit_message>
<xml_diff>
--- a/Draft/Presentation/Run_TestCase/TestCases.xlsx
+++ b/Draft/Presentation/Run_TestCase/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -76,15 +76,9 @@
     <t>linkdev</t>
   </si>
   <si>
-    <t>TestBox</t>
-  </si>
-  <si>
     <t>btnK</t>
   </si>
   <si>
-    <t>btn</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -94,9 +88,6 @@
     <t>Expected</t>
   </si>
   <si>
-    <t>div</t>
-  </si>
-  <si>
     <t>CSS</t>
   </si>
   <si>
@@ -110,6 +101,18 @@
   </si>
   <si>
     <t>Click</t>
+  </si>
+  <si>
+    <t>TextBox</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>Div</t>
+  </si>
+  <si>
+    <t>Assert</t>
   </si>
 </sst>
 </file>
@@ -473,10 +476,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +521,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -535,7 +538,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -549,9 +552,23 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5">
         <v>2</v>
       </c>
     </row>
@@ -567,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +600,7 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -592,10 +609,10 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
         <v>9</v>
@@ -609,16 +626,16 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="G2" t="s">
         <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -626,13 +643,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -640,16 +657,16 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
         <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
       </c>
       <c r="G4" t="s">
         <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add browser variable. add assert logic
</commit_message>
<xml_diff>
--- a/Draft/Presentation/Run_TestCase/TestCases.xlsx
+++ b/Draft/Presentation/Run_TestCase/TestCases.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="1" r:id="rId1"/>
     <sheet name="ExecData" sheetId="2" r:id="rId2"/>
     <sheet name="Elements" sheetId="3" r:id="rId3"/>
+    <sheet name="Lookups" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -61,12 +62,6 @@
     <t>ElementType</t>
   </si>
   <si>
-    <t>Search Google</t>
-  </si>
-  <si>
-    <t>Search for linkdev in google and check the result</t>
-  </si>
-  <si>
     <t>https://www.google.com</t>
   </si>
   <si>
@@ -113,6 +108,33 @@
   </si>
   <si>
     <t>Assert</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>Link Development | A Global Technology Solutions Provider !@#</t>
+  </si>
+  <si>
+    <t>Search Google Positive</t>
+  </si>
+  <si>
+    <t>Search Google Negtive</t>
+  </si>
+  <si>
+    <t>Search for linkdev in google and find the result</t>
+  </si>
+  <si>
+    <t>Search for linkdev in google and fail the result</t>
+  </si>
+  <si>
+    <t>Link Development | A Global Technology Solutions Provider</t>
   </si>
 </sst>
 </file>
@@ -441,32 +463,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -476,15 +515,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
@@ -518,13 +557,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -535,10 +574,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -549,10 +588,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -563,18 +602,78 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5">
+      <c r="G6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D6" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -582,16 +681,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="59.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -600,7 +700,7 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -609,10 +709,10 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>22</v>
       </c>
       <c r="G1" t="s">
         <v>9</v>
@@ -626,16 +726,16 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -643,13 +743,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -657,20 +757,98 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>